<commit_message>
adding new test file
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/Downloads/UCB-BER-DATA-PT-08-2019-U-C/Bootcamp/NBA-Player-Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B43DD85D-B411-364F-96BF-AC4DD0C0F6D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{14D68131-5A6A-CA4D-A261-5F42288E13C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
     <sheet name="minus games" sheetId="2" r:id="rId2"/>
     <sheet name="minus advanced" sheetId="3" r:id="rId3"/>
     <sheet name="advanced" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="81">
   <si>
     <t>g</t>
   </si>
@@ -1109,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -6925,7 +6926,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7531,4 +7532,664 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>48.023255813953497</v>
+      </c>
+      <c r="C2" s="1">
+        <v>72.839080459770102</v>
+      </c>
+      <c r="D2" s="1">
+        <v>74.880434782608603</v>
+      </c>
+      <c r="E2" s="1">
+        <v>26.283018867924401</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44.977272727272698</v>
+      </c>
+      <c r="G2" s="1">
+        <v>53.827586206896498</v>
+      </c>
+      <c r="H2" s="1">
+        <v>70.978723404255305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>35.1860465116279</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9.8735632183908209</v>
+      </c>
+      <c r="D3" s="1">
+        <v>73.663043478260903</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.8867924528301998</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5.9318181818181897</v>
+      </c>
+      <c r="G3" s="1">
+        <v>7.5689655172413897</v>
+      </c>
+      <c r="H3" s="1">
+        <v>48.276595744680797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="1">
+        <v>107.883720930232</v>
+      </c>
+      <c r="C4" s="1">
+        <v>113.068965517241</v>
+      </c>
+      <c r="D4" s="1">
+        <v>113.989130434782</v>
+      </c>
+      <c r="E4" s="1">
+        <v>102.301886792452</v>
+      </c>
+      <c r="F4" s="1">
+        <v>115.72727272727199</v>
+      </c>
+      <c r="G4" s="1">
+        <v>101.568965517241</v>
+      </c>
+      <c r="H4" s="1">
+        <v>110.297872340425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="1">
+        <v>111.418604651162</v>
+      </c>
+      <c r="C5" s="1">
+        <v>110.494252873563</v>
+      </c>
+      <c r="D5" s="1">
+        <v>109.16304347825999</v>
+      </c>
+      <c r="E5" s="1">
+        <v>112</v>
+      </c>
+      <c r="F5" s="1">
+        <v>108.79545454545401</v>
+      </c>
+      <c r="G5" s="1">
+        <v>112.551724137931</v>
+      </c>
+      <c r="H5" s="1">
+        <v>111.74468085106299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="1">
+        <v>14.030232558139501</v>
+      </c>
+      <c r="C6" s="1">
+        <v>13.4954022988505</v>
+      </c>
+      <c r="D6" s="1">
+        <v>18.1999999999999</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10.083018867924499</v>
+      </c>
+      <c r="F6" s="1">
+        <v>14.8295454545454</v>
+      </c>
+      <c r="G6" s="1">
+        <v>10.6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>13.7829787234042</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.54372093023255796</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.56426436781609102</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.57727173913043395</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.50658490566037695</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.58329545454545395</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.50736206896551705</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.55693617021276598</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.32927906976744098</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.39140229885057398</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.33881521739130399</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.41967924528301798</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.27611363636363601</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.40687931034482699</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.36965957446808501</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.23225581395348799</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.243632183908045</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.28280434782608699</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.219452830188679</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.32009090909090898</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.219948275862068</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.237659574468085</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4.7333333333333298</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4.7358695652173903</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3.59245283018867</v>
+      </c>
+      <c r="F10" s="1">
+        <v>7.8068181818181799</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.89482758620689</v>
+      </c>
+      <c r="H10" s="1">
+        <v>5.0319148936170199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="1">
+        <v>16.0697674418604</v>
+      </c>
+      <c r="C11" s="1">
+        <v>14.3735632183908</v>
+      </c>
+      <c r="D11" s="1">
+        <v>16.602173913043401</v>
+      </c>
+      <c r="E11" s="1">
+        <v>12.909433962264099</v>
+      </c>
+      <c r="F11" s="1">
+        <v>20.309090909090902</v>
+      </c>
+      <c r="G11" s="1">
+        <v>12.4672413793103</v>
+      </c>
+      <c r="H11" s="1">
+        <v>15.474468085106301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10.383720930232499</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9.5747126436781596</v>
+      </c>
+      <c r="D12" s="1">
+        <v>10.6989130434782</v>
+      </c>
+      <c r="E12" s="1">
+        <v>8.2075471698113205</v>
+      </c>
+      <c r="F12" s="1">
+        <v>14.040909090909</v>
+      </c>
+      <c r="G12" s="1">
+        <v>7.65</v>
+      </c>
+      <c r="H12" s="1">
+        <v>10.204255319148899</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="1">
+        <v>15.9813953488372</v>
+      </c>
+      <c r="C13" s="1">
+        <v>11.9218390804597</v>
+      </c>
+      <c r="D13" s="1">
+        <v>19.129347826086899</v>
+      </c>
+      <c r="E13" s="1">
+        <v>11.6358490566037</v>
+      </c>
+      <c r="F13" s="1">
+        <v>9.7818181818181795</v>
+      </c>
+      <c r="G13" s="1">
+        <v>14.708620689655101</v>
+      </c>
+      <c r="H13" s="1">
+        <v>11.2489361702127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.54186046511627</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.4264367816091901</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.6217391304347799</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1.54905660377358</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.29772727272727</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1.4310344827586201</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1.43404255319148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.83255813953488</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.81954022988505</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.8836956521739101</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1.34716981132075</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2.875</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.972413793103448</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1.90425531914893</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="1">
+        <v>13.3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>11.183908045977001</v>
+      </c>
+      <c r="D16" s="1">
+        <v>12.1467391304347</v>
+      </c>
+      <c r="E16" s="1">
+        <v>12.377358490565999</v>
+      </c>
+      <c r="F16" s="1">
+        <v>12.590909090908999</v>
+      </c>
+      <c r="G16" s="1">
+        <v>12.7844827586206</v>
+      </c>
+      <c r="H16" s="1">
+        <v>11.582978723404199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="1">
+        <v>19.320930232558101</v>
+      </c>
+      <c r="C17" s="1">
+        <v>17.1149425287356</v>
+      </c>
+      <c r="D17" s="1">
+        <v>22.796739130434698</v>
+      </c>
+      <c r="E17" s="1">
+        <v>16.898113207547102</v>
+      </c>
+      <c r="F17" s="1">
+        <v>16.190909090908999</v>
+      </c>
+      <c r="G17" s="1">
+        <v>18.722413793103399</v>
+      </c>
+      <c r="H17" s="1">
+        <v>18.253191489361701</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.81627906976744102</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.62643678160919</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3.84021739130434</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2.6415094339622601E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.81818181818181801</v>
+      </c>
+      <c r="G18" s="1">
+        <v>4.6551724137930899E-2</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1.63829787234042</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.0953488372093001</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.52758620689655</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2.7423913043478199</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.31132075471698101</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.71363636363636296</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.71379310344827596</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1.5702127659574401</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.9186046511627901</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.1482758620689602</v>
+      </c>
+      <c r="D20" s="1">
+        <v>6.5836956521739101</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.33396226415094299</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1.53863636363636</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.76896551724137796</v>
+      </c>
+      <c r="H20" s="1">
+        <v>3.1914893617021201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="1">
+        <v>7.7023255813953403E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.101206896551724</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.13495652173913</v>
+      </c>
+      <c r="E21" s="1">
+        <v>4.3660377358490501E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.12186363636363599</v>
+      </c>
+      <c r="G21" s="1">
+        <v>3.7879310344827603E-2</v>
+      </c>
+      <c r="H21" s="1">
+        <v>8.5489361702127606E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="1">
+        <v>-0.86279069767441796</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-0.50804597701149401</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.6728260869565199</v>
+      </c>
+      <c r="E22" s="1">
+        <v>-2.74339622641509</v>
+      </c>
+      <c r="F22" s="1">
+        <v>-1.3272727272727201</v>
+      </c>
+      <c r="G22" s="1">
+        <v>-2.4379310344827498</v>
+      </c>
+      <c r="H22" s="1">
+        <v>-0.59361702127659499</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="1">
+        <v>-5.8139534883720902E-2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>-2.6436781609195301E-2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.58913043478260796</v>
+      </c>
+      <c r="E23" s="1">
+        <v>-0.98490566037735805</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.77954545454545399</v>
+      </c>
+      <c r="G23" s="1">
+        <v>-1.35689655172413</v>
+      </c>
+      <c r="H23" s="1">
+        <v>-4.4680851063829699E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="1">
+        <v>-0.93720930232558097</v>
+      </c>
+      <c r="C24" s="1">
+        <v>-0.53678160919540197</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2.25652173913043</v>
+      </c>
+      <c r="E24" s="1">
+        <v>-3.7264150943396199</v>
+      </c>
+      <c r="F24" s="1">
+        <v>-0.53863636363636302</v>
+      </c>
+      <c r="G24" s="1">
+        <v>-3.7948275862068899</v>
+      </c>
+      <c r="H24" s="1">
+        <v>-0.64893617021276595</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.32093023255813902</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.57356321839080404</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2.5402173913043402</v>
+      </c>
+      <c r="E25" s="1">
+        <v>-0.152830188679244</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.20909090909090899</v>
+      </c>
+      <c r="G25" s="1">
+        <v>-0.35689655172413698</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.60638297872340396</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>